<commit_message>
a ton of models
</commit_message>
<xml_diff>
--- a/experiments/lidar_mocap/HCN11/best_accuracy_series.xlsx
+++ b/experiments/lidar_mocap/HCN11/best_accuracy_series.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:U2"/>
+  <dimension ref="B1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,135 +457,31 @@
           <t>epoch350</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>epoch400</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>epoch450</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>epoch500</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>epoch550</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>epoch600</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>epoch650</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>epoch700</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>epoch750</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>epoch800</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>epoch850</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>epoch900</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>epoch950</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>epoch1000</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="B2" t="n">
-        <v>86.44448146224022</v>
+        <v>86.05385646224022</v>
       </c>
       <c r="C2" t="n">
-        <v>86.44448146224022</v>
+        <v>86.05385646224022</v>
       </c>
       <c r="D2" t="n">
-        <v>86.44448146224022</v>
+        <v>86.05385646224022</v>
       </c>
       <c r="E2" t="n">
-        <v>86.44448146224022</v>
+        <v>86.05385646224022</v>
       </c>
       <c r="F2" t="n">
-        <v>86.44448146224022</v>
+        <v>85.23936197161674</v>
       </c>
       <c r="G2" t="n">
-        <v>86.44448146224022</v>
+        <v>85.23936197161674</v>
       </c>
       <c r="H2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="I2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="J2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="K2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="L2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="M2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="N2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="O2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="P2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="R2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="S2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="T2" t="n">
-        <v>86.44448146224022</v>
-      </c>
-      <c r="U2" t="n">
-        <v>86.44448146224022</v>
+        <v>85.23936197161674</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>